<commit_message>
chore: sync repo with latest training pipeline, results reorg, and artifacts
</commit_message>
<xml_diff>
--- a/data/raw/ECOLAND_20250703_cycle1.xlsx
+++ b/data/raw/ECOLAND_20250703_cycle1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnf\Desktop\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnf\Desktop\D3QN\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD248BD-2CF2-43C6-8306-5CE615CA815B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8EA50F-6811-4293-9B43-5DF39A44B141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -240,45 +240,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1047750</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2800350" cy="4152900"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image1.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -479,7 +440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -2737,7 +2698,6 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>